<commit_message>
ratio template: change label workerstation name
</commit_message>
<xml_diff>
--- a/IncaArt/IncaArt/Resources/Excel/new_ratios.xlsx
+++ b/IncaArt/IncaArt/Resources/Excel/new_ratios.xlsx
@@ -21,24 +21,9 @@
     <t>Trabajador</t>
   </si>
   <si>
-    <t>MoldeadoC</t>
-  </si>
-  <si>
-    <t>PintandoC</t>
-  </si>
-  <si>
-    <t>HorneadoC</t>
-  </si>
-  <si>
     <t>Tallado</t>
   </si>
   <si>
-    <t>MoldeadoR</t>
-  </si>
-  <si>
-    <t>PintadoR</t>
-  </si>
-  <si>
     <t>Ratios de Trabajadores</t>
   </si>
   <si>
@@ -55,6 +40,21 @@
   </si>
   <si>
     <t>Cantidad producida por hora</t>
+  </si>
+  <si>
+    <t>Moldeado Cerámico</t>
+  </si>
+  <si>
+    <t>Pintando Cerámico</t>
+  </si>
+  <si>
+    <t>Horneado Cerámico</t>
+  </si>
+  <si>
+    <t>Moldeado Retablo</t>
+  </si>
+  <si>
+    <t>Pintado Retablo</t>
   </si>
 </sst>
 </file>
@@ -173,6 +173,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -186,12 +192,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,7 +503,7 @@
   <dimension ref="A2:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -512,111 +512,111 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="5"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="8"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>